<commit_message>
pipe heat loss calculation updated; pipe pressure loss calculation updated; pipe costs added; views added and updated; Code reformatted
</commit_message>
<xml_diff>
--- a/resources/parameters/DN_Rohrdurchmesser.xlsx
+++ b/resources/parameters/DN_Rohrdurchmesser.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\PycharmProjects\PBE1\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\PycharmProjects\pbe1\resources\parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9020635A-EC69-42DC-B8C2-204601729F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0416814-AD71-4DBA-8E6B-2E343C3C655A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="2730" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{AB66346F-2E87-47D8-A865-C4A8F39C8C07}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AB66346F-2E87-47D8-A865-C4A8F39C8C07}"/>
   </bookViews>
   <sheets>
     <sheet name="PMR" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="327">
   <si>
     <t>Stahlmediumrohr; Quelle: SET</t>
   </si>
@@ -1010,13 +1010,29 @@
   </si>
   <si>
     <t>0.349</t>
+  </si>
+  <si>
+    <t>Kosten Straße CHF/m</t>
+  </si>
+  <si>
+    <t>Aufschlag (30%)</t>
+  </si>
+  <si>
+    <t>Kosten Straße €/m</t>
+  </si>
+  <si>
+    <t>Umrechnung CHF in €</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="170" formatCode="_-* #,##0.00\ [$CHF]_-;\-* #,##0.00\ [$CHF]_-;_-* &quot;-&quot;??\ [$CHF]_-;_-@_-"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1026,6 +1042,13 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1050,10 +1073,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1063,11 +1087,34 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Währung" xfId="1" builtinId="4"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="63">
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="_-* #,##0.00\ [$CHF]_-;\-* #,##0.00\ [$CHF]_-;_-* &quot;-&quot;??\ [$CHF]_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="_-* #,##0.00\ [$CHF]_-;\-* #,##0.00\ [$CHF]_-;_-* &quot;-&quot;??\ [$CHF]_-;_-@_-"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1075,34 +1122,34 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="170" formatCode="_-* #,##0.00\ [$CHF]_-;\-* #,##0.00\ [$CHF]_-;_-* &quot;-&quot;??\ [$CHF]_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="170" formatCode="_-* #,##0.00\ [$CHF]_-;\-* #,##0.00\ [$CHF]_-;_-* &quot;-&quot;??\ [$CHF]_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="170" formatCode="_-* #,##0.00\ [$CHF]_-;\-* #,##0.00\ [$CHF]_-;_-* &quot;-&quot;??\ [$CHF]_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="170" formatCode="_-* #,##0.00\ [$CHF]_-;\-* #,##0.00\ [$CHF]_-;_-* &quot;-&quot;??\ [$CHF]_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="170" formatCode="_-* #,##0.00\ [$CHF]_-;\-* #,##0.00\ [$CHF]_-;_-* &quot;-&quot;??\ [$CHF]_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="170" formatCode="_-* #,##0.00\ [$CHF]_-;\-* #,##0.00\ [$CHF]_-;_-* &quot;-&quot;??\ [$CHF]_-;_-@_-"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1144,6 +1191,36 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -1175,9 +1252,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1226,80 +1300,112 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{15877BAD-33A9-4A96-AF77-5CFECF0EFFE8}" name="Tabelle1" displayName="Tabelle1" ref="A1:K11" totalsRowShown="0" headerRowDxfId="47">
-  <autoFilter ref="A1:K11" xr:uid="{15877BAD-33A9-4A96-AF77-5CFECF0EFFE8}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{908F630C-F4FD-4F3D-B2EC-C66F74879A84}" name="Nennweite" dataDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{1E274E17-72A6-4602-A119-23580B43DC88}" name="Aussendurchmesser" dataDxfId="45"/>
-    <tableColumn id="3" xr3:uid="{60FE333F-F948-4505-BCEC-1443D6A0C0AE}" name="Wandstärke" dataDxfId="44"/>
-    <tableColumn id="4" xr3:uid="{6424EB7A-F472-463D-9530-1DE0A388382E}" name="Innendurchmesser" dataDxfId="43"/>
-    <tableColumn id="5" xr3:uid="{99D72574-F9ED-4F8B-9B47-FD9A8A208310}" name="Volumen Innenrohr" dataDxfId="42"/>
-    <tableColumn id="6" xr3:uid="{F90611F3-DCE0-4074-A666-CD784A1B01A4}" name="DS1-D" dataDxfId="41"/>
-    <tableColumn id="7" xr3:uid="{E6D28259-34E9-48CE-AD47-82FA4C2329CB}" name="DS2-D" dataDxfId="40"/>
-    <tableColumn id="8" xr3:uid="{4086A163-4AA1-4EFB-A7A6-BB90D6C96806}" name="DS3-D" dataDxfId="39"/>
-    <tableColumn id="9" xr3:uid="{B73A8171-D6E7-4A91-B2CE-07E64319D57D}" name="DS1-W" dataDxfId="38"/>
-    <tableColumn id="10" xr3:uid="{14D8FE8D-C8D4-4987-81B2-A0FB61AA23BC}" name="DS2-W" dataDxfId="37"/>
-    <tableColumn id="11" xr3:uid="{33F2FDBD-5664-4D74-A508-E7C61EC66D75}" name="DS3-W" dataDxfId="36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{15877BAD-33A9-4A96-AF77-5CFECF0EFFE8}" name="Tabelle1" displayName="Tabelle1" ref="A1:O11" totalsRowShown="0" headerRowDxfId="62">
+  <autoFilter ref="A1:O11" xr:uid="{15877BAD-33A9-4A96-AF77-5CFECF0EFFE8}"/>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{908F630C-F4FD-4F3D-B2EC-C66F74879A84}" name="Nennweite" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{1E274E17-72A6-4602-A119-23580B43DC88}" name="Aussendurchmesser" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{60FE333F-F948-4505-BCEC-1443D6A0C0AE}" name="Wandstärke" dataDxfId="59"/>
+    <tableColumn id="4" xr3:uid="{6424EB7A-F472-463D-9530-1DE0A388382E}" name="Innendurchmesser" dataDxfId="58"/>
+    <tableColumn id="5" xr3:uid="{99D72574-F9ED-4F8B-9B47-FD9A8A208310}" name="Volumen Innenrohr" dataDxfId="57"/>
+    <tableColumn id="6" xr3:uid="{F90611F3-DCE0-4074-A666-CD784A1B01A4}" name="DS1-D" dataDxfId="56"/>
+    <tableColumn id="7" xr3:uid="{E6D28259-34E9-48CE-AD47-82FA4C2329CB}" name="DS2-D" dataDxfId="55"/>
+    <tableColumn id="8" xr3:uid="{4086A163-4AA1-4EFB-A7A6-BB90D6C96806}" name="DS3-D" dataDxfId="54"/>
+    <tableColumn id="9" xr3:uid="{B73A8171-D6E7-4A91-B2CE-07E64319D57D}" name="DS1-W" dataDxfId="53"/>
+    <tableColumn id="10" xr3:uid="{14D8FE8D-C8D4-4987-81B2-A0FB61AA23BC}" name="DS2-W" dataDxfId="52"/>
+    <tableColumn id="11" xr3:uid="{33F2FDBD-5664-4D74-A508-E7C61EC66D75}" name="DS3-W" dataDxfId="15"/>
+    <tableColumn id="12" xr3:uid="{37459105-C451-4F9D-B519-D3E315BCDE9D}" name="Kosten Straße CHF/m" dataDxfId="14"/>
+    <tableColumn id="13" xr3:uid="{CB255951-4ECE-4852-83B6-2E378B14309C}" name="Aufschlag (30%)" dataDxfId="13">
+      <calculatedColumnFormula>Tabelle1[[#This Row],[Kosten Straße CHF/m]]*0.3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="14" xr3:uid="{C19B7817-BE53-47E0-9388-E9CA95C9A81E}" name="Umrechnung CHF in €" dataDxfId="12"/>
+    <tableColumn id="15" xr3:uid="{DCA4CFAC-4277-413E-B22A-ED16D181E94A}" name="Kosten Straße €/m" dataDxfId="0">
+      <calculatedColumnFormula>ROUND((Tabelle1[[#This Row],[Kosten Straße CHF/m]]+Tabelle1[[#This Row],[Aufschlag (30%)]])*Tabelle1[[#This Row],[Umrechnung CHF in €]],2)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FBAF5C86-0712-43DF-97C0-EC70371C9FF1}" name="Tabelle13" displayName="Tabelle13" ref="A1:K6" totalsRowShown="0" headerRowDxfId="35">
-  <autoFilter ref="A1:K6" xr:uid="{15877BAD-33A9-4A96-AF77-5CFECF0EFFE8}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{F71AEB89-AC77-4385-AE31-EB092DC7C2BB}" name="Nennweite" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{240743CB-A45B-4DE4-8809-9E38B4DA8F99}" name="Aussendurchmesser" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{75E99B1E-54F8-4D6E-B04D-54685399DA7C}" name="Wandstärke" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{3B82ADD7-00FA-426A-9134-2D76B34B1934}" name="Innendurchmesser" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{55EA12A3-958F-4DC3-BD7F-4230E433E8CD}" name="Volumen Innenrohr" dataDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{12463EC1-0E22-4419-9805-2D19A98B148E}" name="DS1-D" dataDxfId="29"/>
-    <tableColumn id="7" xr3:uid="{DAF428DC-5F65-4016-9536-9EE262A4E257}" name="DS2-D" dataDxfId="28"/>
-    <tableColumn id="8" xr3:uid="{A0BFABE6-8F52-4808-ADC0-A516F6034795}" name="DS3-D" dataDxfId="27"/>
-    <tableColumn id="9" xr3:uid="{63949EA0-FCC7-4F1C-9943-05CFF007FC50}" name="DS1-W" dataDxfId="26"/>
-    <tableColumn id="10" xr3:uid="{0ECEDF08-9602-4AF0-BC89-9A3056007D38}" name="DS2-W" dataDxfId="25"/>
-    <tableColumn id="11" xr3:uid="{15A4E1BE-6CA2-40A6-BD01-64824D06203C}" name="DS3-W" dataDxfId="24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FBAF5C86-0712-43DF-97C0-EC70371C9FF1}" name="Tabelle13" displayName="Tabelle13" ref="A1:O6" totalsRowShown="0" headerRowDxfId="51">
+  <autoFilter ref="A1:O6" xr:uid="{15877BAD-33A9-4A96-AF77-5CFECF0EFFE8}"/>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{F71AEB89-AC77-4385-AE31-EB092DC7C2BB}" name="Nennweite" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{240743CB-A45B-4DE4-8809-9E38B4DA8F99}" name="Aussendurchmesser" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{75E99B1E-54F8-4D6E-B04D-54685399DA7C}" name="Wandstärke" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{3B82ADD7-00FA-426A-9134-2D76B34B1934}" name="Innendurchmesser" dataDxfId="47"/>
+    <tableColumn id="5" xr3:uid="{55EA12A3-958F-4DC3-BD7F-4230E433E8CD}" name="Volumen Innenrohr" dataDxfId="46"/>
+    <tableColumn id="6" xr3:uid="{12463EC1-0E22-4419-9805-2D19A98B148E}" name="DS1-D" dataDxfId="45"/>
+    <tableColumn id="7" xr3:uid="{DAF428DC-5F65-4016-9536-9EE262A4E257}" name="DS2-D" dataDxfId="44"/>
+    <tableColumn id="8" xr3:uid="{A0BFABE6-8F52-4808-ADC0-A516F6034795}" name="DS3-D" dataDxfId="43"/>
+    <tableColumn id="9" xr3:uid="{63949EA0-FCC7-4F1C-9943-05CFF007FC50}" name="DS1-W" dataDxfId="42"/>
+    <tableColumn id="10" xr3:uid="{0ECEDF08-9602-4AF0-BC89-9A3056007D38}" name="DS2-W" dataDxfId="41"/>
+    <tableColumn id="11" xr3:uid="{15A4E1BE-6CA2-40A6-BD01-64824D06203C}" name="DS3-W" dataDxfId="18"/>
+    <tableColumn id="12" xr3:uid="{D793674F-C3EE-44A4-8662-0D9A418F3903}" name="Kosten Straße CHF/m" dataDxfId="17" dataCellStyle="Währung"/>
+    <tableColumn id="13" xr3:uid="{75305D35-BE02-4164-95C9-09A077293FBF}" name="Aufschlag (30%)" dataDxfId="16">
+      <calculatedColumnFormula>Tabelle13[[#This Row],[Kosten Straße CHF/m]]*0.3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="14" xr3:uid="{50E5C238-45F3-4FFA-B258-6DD799177B5E}" name="Umrechnung CHF in €"/>
+    <tableColumn id="15" xr3:uid="{FC0FD09D-79B0-409E-AFE5-405E2E141B07}" name="Kosten Straße €/m" dataDxfId="1">
+      <calculatedColumnFormula>ROUND((Tabelle13[[#This Row],[Kosten Straße CHF/m]]+Tabelle13[[#This Row],[Aufschlag (30%)]])*Tabelle13[[#This Row],[Umrechnung CHF in €]],2)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{99A13040-C4A2-467E-BC65-C3AD509682A7}" name="Tabelle145" displayName="Tabelle145" ref="A1:K23" totalsRowShown="0" headerRowDxfId="23">
-  <autoFilter ref="A1:K23" xr:uid="{15877BAD-33A9-4A96-AF77-5CFECF0EFFE8}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{D9CBA266-53F4-4CFD-85CA-D0B74F023628}" name="Nennweite" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{5064B2E4-F33A-4445-8068-6CAB4759DE40}" name="Aussendurchmesser" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{08CD9950-3524-452B-9FFF-E4EDDC4FB98F}" name="Wandstärke" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{5FC5A318-3EDF-4FFC-A668-ECF888D58E33}" name="Innendurchmesser" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{41ADB498-852B-4581-BDD8-92BEA139B453}" name="Volumen Innenrohr" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{F086323B-7624-44FE-BB6A-EE19A1033421}" name="DS1-D" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{B2802424-1844-4487-993F-72F92AE821D6}" name="DS2-D" dataDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{63C80DBD-44F6-40E5-BF3D-31285DCE8FA8}" name="DS3-D" dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{E1796E0B-CEE5-48BB-B1FD-3FF1445D5EC5}" name="DS1-W" dataDxfId="14"/>
-    <tableColumn id="10" xr3:uid="{798B330F-6637-4622-90B9-1ADC139A7CDF}" name="DS2-W" dataDxfId="13"/>
-    <tableColumn id="11" xr3:uid="{A7853943-AA5F-45F8-AA23-59EB7DE71E05}" name="DS3-W" dataDxfId="12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{99A13040-C4A2-467E-BC65-C3AD509682A7}" name="Tabelle145" displayName="Tabelle145" ref="A1:O23" totalsRowShown="0" headerRowDxfId="40">
+  <autoFilter ref="A1:O23" xr:uid="{15877BAD-33A9-4A96-AF77-5CFECF0EFFE8}"/>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{D9CBA266-53F4-4CFD-85CA-D0B74F023628}" name="Nennweite" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{5064B2E4-F33A-4445-8068-6CAB4759DE40}" name="Aussendurchmesser" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{08CD9950-3524-452B-9FFF-E4EDDC4FB98F}" name="Wandstärke" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{5FC5A318-3EDF-4FFC-A668-ECF888D58E33}" name="Innendurchmesser" dataDxfId="36"/>
+    <tableColumn id="5" xr3:uid="{41ADB498-852B-4581-BDD8-92BEA139B453}" name="Volumen Innenrohr" dataDxfId="35"/>
+    <tableColumn id="6" xr3:uid="{F086323B-7624-44FE-BB6A-EE19A1033421}" name="DS1-D" dataDxfId="34"/>
+    <tableColumn id="7" xr3:uid="{B2802424-1844-4487-993F-72F92AE821D6}" name="DS2-D" dataDxfId="33"/>
+    <tableColumn id="8" xr3:uid="{63C80DBD-44F6-40E5-BF3D-31285DCE8FA8}" name="DS3-D" dataDxfId="32"/>
+    <tableColumn id="9" xr3:uid="{E1796E0B-CEE5-48BB-B1FD-3FF1445D5EC5}" name="DS1-W" dataDxfId="31"/>
+    <tableColumn id="10" xr3:uid="{798B330F-6637-4622-90B9-1ADC139A7CDF}" name="DS2-W" dataDxfId="30"/>
+    <tableColumn id="11" xr3:uid="{A7853943-AA5F-45F8-AA23-59EB7DE71E05}" name="DS3-W" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{56D917F5-80B2-4617-B651-1778339C6C65}" name="Kosten Straße CHF/m" dataDxfId="10"/>
+    <tableColumn id="13" xr3:uid="{37E275FB-4EDE-48AE-B769-AFAC96F1DA08}" name="Aufschlag (30%)" dataDxfId="9">
+      <calculatedColumnFormula>Tabelle145[[#This Row],[Kosten Straße CHF/m]]*0.3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="14" xr3:uid="{0656AAEA-ADE0-430E-88BB-D11E9CC333D0}" name="Umrechnung CHF in €" dataDxfId="7"/>
+    <tableColumn id="15" xr3:uid="{D8E987FF-D19C-43DC-876B-1A0AF31C7DA2}" name="Kosten Straße €/m" dataDxfId="8">
+      <calculatedColumnFormula>ROUND((Tabelle145[[#This Row],[Kosten Straße CHF/m]]+Tabelle145[[#This Row],[Aufschlag (30%)]])*Tabelle145[[#This Row],[Umrechnung CHF in €]],2)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C0B41E0A-3896-44FB-B5C2-A4FA08ED7479}" name="Tabelle14" displayName="Tabelle14" ref="A1:K12" totalsRowShown="0" headerRowDxfId="11">
-  <autoFilter ref="A1:K12" xr:uid="{15877BAD-33A9-4A96-AF77-5CFECF0EFFE8}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{CB5045F2-D781-488D-B0AD-40BFF665368B}" name="Nennweite" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{B752C930-9065-43FF-8824-039EEAE790F1}" name="Aussendurchmesser" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{5C0A0490-A7F9-451B-9DB2-CDB82CBD6D59}" name="Wandstärke" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{32AF510A-66DE-495D-A2D3-24936E4F4143}" name="Innendurchmesser" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{38BDC2F5-0953-4FE2-BE64-8D78C98E9CB9}" name="Volumen Innenrohr" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{C95A10C9-2B4B-474C-ABC4-0EAFBCE178CF}" name="DS1-D" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{F7B85530-5403-4165-8AE6-566B0E38994A}" name="DS2-D" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{03E7F748-55FA-4A19-A944-36403118DDCD}" name="DS3-D" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{D486F602-BF9D-489B-A322-C758AE511255}" name="DS1-W" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{D2EF9A28-4586-49C7-BBC3-493A6EEC757F}" name="DS2-W" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{8C845D78-B204-4D0F-A02B-36C964C5F84C}" name="DS3-W" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C0B41E0A-3896-44FB-B5C2-A4FA08ED7479}" name="Tabelle14" displayName="Tabelle14" ref="A1:O12" totalsRowShown="0" headerRowDxfId="29">
+  <autoFilter ref="A1:O12" xr:uid="{15877BAD-33A9-4A96-AF77-5CFECF0EFFE8}"/>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{CB5045F2-D781-488D-B0AD-40BFF665368B}" name="Nennweite" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{B752C930-9065-43FF-8824-039EEAE790F1}" name="Aussendurchmesser" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{5C0A0490-A7F9-451B-9DB2-CDB82CBD6D59}" name="Wandstärke" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{32AF510A-66DE-495D-A2D3-24936E4F4143}" name="Innendurchmesser" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{38BDC2F5-0953-4FE2-BE64-8D78C98E9CB9}" name="Volumen Innenrohr" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{C95A10C9-2B4B-474C-ABC4-0EAFBCE178CF}" name="DS1-D" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{F7B85530-5403-4165-8AE6-566B0E38994A}" name="DS2-D" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{03E7F748-55FA-4A19-A944-36403118DDCD}" name="DS3-D" dataDxfId="21"/>
+    <tableColumn id="9" xr3:uid="{D486F602-BF9D-489B-A322-C758AE511255}" name="DS1-W" dataDxfId="20"/>
+    <tableColumn id="10" xr3:uid="{D2EF9A28-4586-49C7-BBC3-493A6EEC757F}" name="DS2-W" dataDxfId="19"/>
+    <tableColumn id="11" xr3:uid="{8C845D78-B204-4D0F-A02B-36C964C5F84C}" name="DS3-W" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{D9F92F9B-D82A-480B-AAE2-73AD4E45FCB2}" name="Kosten Straße CHF/m" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{8EA9B582-A804-4652-BAB7-F9566859BAED}" name="Aufschlag (30%)" dataDxfId="4">
+      <calculatedColumnFormula>Tabelle14[[#This Row],[Kosten Straße CHF/m]]*0.3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="14" xr3:uid="{CD307070-D372-4EE0-B6D6-9242E4186153}" name="Umrechnung CHF in €" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{88CB6F5C-4892-44CB-93D9-9B545D03C56A}" name="Kosten Straße €/m" dataDxfId="3">
+      <calculatedColumnFormula>ROUND((Tabelle14[[#This Row],[Kosten Straße CHF/m]]+Tabelle14[[#This Row],[Aufschlag (30%)]])*Tabelle14[[#This Row],[Umrechnung CHF in €]],2)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1602,10 +1708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B2F2E02-ABF7-4DA8-8783-089E5941DC2E}">
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1616,9 +1722,13 @@
     <col min="4" max="4" width="19.42578125" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" customWidth="1"/>
     <col min="6" max="11" width="12.140625" customWidth="1"/>
+    <col min="12" max="12" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>270</v>
       </c>
@@ -1652,8 +1762,20 @@
       <c r="K1" s="4" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>164</v>
       </c>
@@ -1687,8 +1809,22 @@
       <c r="K2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="6">
+        <v>346</v>
+      </c>
+      <c r="M2" s="7">
+        <f>Tabelle1[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>103.8</v>
+      </c>
+      <c r="N2" s="8">
+        <v>1.02</v>
+      </c>
+      <c r="O2" s="5">
+        <f>ROUND((Tabelle1[[#This Row],[Kosten Straße CHF/m]]+Tabelle1[[#This Row],[Aufschlag (30%)]])*Tabelle1[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>458.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>170</v>
       </c>
@@ -1722,8 +1858,23 @@
       <c r="K3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="6">
+        <v>358</v>
+      </c>
+      <c r="M3" s="7">
+        <f>Tabelle1[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>107.39999999999999</v>
+      </c>
+      <c r="N3" s="8">
+        <f>$N$2</f>
+        <v>1.02</v>
+      </c>
+      <c r="O3" s="5">
+        <f>ROUND((Tabelle1[[#This Row],[Kosten Straße CHF/m]]+Tabelle1[[#This Row],[Aufschlag (30%)]])*Tabelle1[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>474.71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>172</v>
       </c>
@@ -1757,8 +1908,23 @@
       <c r="K4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="6">
+        <v>406</v>
+      </c>
+      <c r="M4" s="7">
+        <f>Tabelle1[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>121.8</v>
+      </c>
+      <c r="N4" s="8">
+        <f t="shared" ref="N4:N11" si="0">$N$2</f>
+        <v>1.02</v>
+      </c>
+      <c r="O4" s="5">
+        <f>ROUND((Tabelle1[[#This Row],[Kosten Straße CHF/m]]+Tabelle1[[#This Row],[Aufschlag (30%)]])*Tabelle1[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>538.36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>175</v>
       </c>
@@ -1792,8 +1958,23 @@
       <c r="K5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="6">
+        <v>423</v>
+      </c>
+      <c r="M5" s="7">
+        <f>Tabelle1[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>126.89999999999999</v>
+      </c>
+      <c r="N5" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O5" s="5">
+        <f>ROUND((Tabelle1[[#This Row],[Kosten Straße CHF/m]]+Tabelle1[[#This Row],[Aufschlag (30%)]])*Tabelle1[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>560.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>177</v>
       </c>
@@ -1827,8 +2008,23 @@
       <c r="K6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="6">
+        <v>548</v>
+      </c>
+      <c r="M6" s="7">
+        <f>Tabelle1[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>164.4</v>
+      </c>
+      <c r="N6" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O6" s="5">
+        <f>ROUND((Tabelle1[[#This Row],[Kosten Straße CHF/m]]+Tabelle1[[#This Row],[Aufschlag (30%)]])*Tabelle1[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>726.65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>181</v>
       </c>
@@ -1862,8 +2058,23 @@
       <c r="K7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="7">
+        <v>618</v>
+      </c>
+      <c r="M7" s="7">
+        <f>Tabelle1[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>185.4</v>
+      </c>
+      <c r="N7" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O7" s="5">
+        <f>ROUND((Tabelle1[[#This Row],[Kosten Straße CHF/m]]+Tabelle1[[#This Row],[Aufschlag (30%)]])*Tabelle1[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>819.47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>184</v>
       </c>
@@ -1897,8 +2108,23 @@
       <c r="K8" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="7">
+        <v>708</v>
+      </c>
+      <c r="M8" s="7">
+        <f>Tabelle1[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>212.4</v>
+      </c>
+      <c r="N8" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O8" s="5">
+        <f>ROUND((Tabelle1[[#This Row],[Kosten Straße CHF/m]]+Tabelle1[[#This Row],[Aufschlag (30%)]])*Tabelle1[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>938.81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>188</v>
       </c>
@@ -1932,8 +2158,23 @@
       <c r="K9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="7">
+        <v>762</v>
+      </c>
+      <c r="M9" s="7">
+        <f>Tabelle1[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>228.6</v>
+      </c>
+      <c r="N9" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O9" s="5">
+        <f>ROUND((Tabelle1[[#This Row],[Kosten Straße CHF/m]]+Tabelle1[[#This Row],[Aufschlag (30%)]])*Tabelle1[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>1010.41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>169</v>
       </c>
@@ -1967,8 +2208,23 @@
       <c r="K10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="7">
+        <v>816</v>
+      </c>
+      <c r="M10" s="7">
+        <f>Tabelle1[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>244.79999999999998</v>
+      </c>
+      <c r="N10" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O10" s="5">
+        <f>ROUND((Tabelle1[[#This Row],[Kosten Straße CHF/m]]+Tabelle1[[#This Row],[Aufschlag (30%)]])*Tabelle1[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>1082.02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>194</v>
       </c>
@@ -2002,8 +2258,23 @@
       <c r="K11" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="7">
+        <v>870</v>
+      </c>
+      <c r="M11" s="7">
+        <f>Tabelle1[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>261</v>
+      </c>
+      <c r="N11" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O11" s="5">
+        <f>ROUND((Tabelle1[[#This Row],[Kosten Straße CHF/m]]+Tabelle1[[#This Row],[Aufschlag (30%)]])*Tabelle1[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>1153.6199999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -2014,7 +2285,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -2095,10 +2366,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB7C6AD9-AC1B-4FBD-B1DD-E06A769DA67F}">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2109,9 +2380,13 @@
     <col min="4" max="4" width="19.42578125" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" customWidth="1"/>
     <col min="6" max="11" width="12.140625" customWidth="1"/>
+    <col min="12" max="12" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>270</v>
       </c>
@@ -2145,8 +2420,20 @@
       <c r="K1" s="4" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L1" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>164</v>
       </c>
@@ -2180,8 +2467,22 @@
       <c r="K2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L2" s="6">
+        <v>278</v>
+      </c>
+      <c r="M2" s="7">
+        <f>Tabelle13[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>83.399999999999991</v>
+      </c>
+      <c r="N2">
+        <v>1.02</v>
+      </c>
+      <c r="O2" s="5">
+        <f>ROUND((Tabelle13[[#This Row],[Kosten Straße CHF/m]]+Tabelle13[[#This Row],[Aufschlag (30%)]])*Tabelle13[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>368.63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>170</v>
       </c>
@@ -2215,8 +2516,23 @@
       <c r="K3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L3" s="6">
+        <v>322</v>
+      </c>
+      <c r="M3" s="7">
+        <f>Tabelle13[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>96.6</v>
+      </c>
+      <c r="N3">
+        <f>$N$2</f>
+        <v>1.02</v>
+      </c>
+      <c r="O3" s="5">
+        <f>ROUND((Tabelle13[[#This Row],[Kosten Straße CHF/m]]+Tabelle13[[#This Row],[Aufschlag (30%)]])*Tabelle13[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>426.97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>172</v>
       </c>
@@ -2250,8 +2566,23 @@
       <c r="K4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L4" s="6">
+        <v>350</v>
+      </c>
+      <c r="M4" s="7">
+        <f>Tabelle13[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>105</v>
+      </c>
+      <c r="N4">
+        <f t="shared" ref="N4:N6" si="0">$N$2</f>
+        <v>1.02</v>
+      </c>
+      <c r="O4" s="5">
+        <f>ROUND((Tabelle13[[#This Row],[Kosten Straße CHF/m]]+Tabelle13[[#This Row],[Aufschlag (30%)]])*Tabelle13[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>464.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>175</v>
       </c>
@@ -2285,8 +2616,23 @@
       <c r="K5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L5" s="6">
+        <v>415</v>
+      </c>
+      <c r="M5" s="7">
+        <f>Tabelle13[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>124.5</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O5" s="5">
+        <f>ROUND((Tabelle13[[#This Row],[Kosten Straße CHF/m]]+Tabelle13[[#This Row],[Aufschlag (30%)]])*Tabelle13[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>550.29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>50</v>
       </c>
@@ -2320,8 +2666,23 @@
       <c r="K6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L6" s="6">
+        <v>452</v>
+      </c>
+      <c r="M6" s="7">
+        <f>Tabelle13[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>135.6</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O6" s="5">
+        <f>ROUND((Tabelle13[[#This Row],[Kosten Straße CHF/m]]+Tabelle13[[#This Row],[Aufschlag (30%)]])*Tabelle13[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>599.35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -2336,7 +2697,7 @@
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -2351,7 +2712,7 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -2366,7 +2727,7 @@
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -2391,10 +2752,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{008DF0A2-A46D-4661-9C6A-A70ABEB52FB4}">
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2405,9 +2766,13 @@
     <col min="4" max="4" width="19.42578125" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" customWidth="1"/>
     <col min="6" max="11" width="12.140625" customWidth="1"/>
+    <col min="12" max="12" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>270</v>
       </c>
@@ -2441,8 +2806,20 @@
       <c r="K1" s="4" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>164</v>
       </c>
@@ -2476,8 +2853,22 @@
       <c r="K2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="6">
+        <v>473</v>
+      </c>
+      <c r="M2" s="7">
+        <f>Tabelle145[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>141.9</v>
+      </c>
+      <c r="N2" s="8">
+        <v>1.02</v>
+      </c>
+      <c r="O2" s="5">
+        <f>ROUND((Tabelle145[[#This Row],[Kosten Straße CHF/m]]+Tabelle145[[#This Row],[Aufschlag (30%)]])*Tabelle145[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>627.20000000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>170</v>
       </c>
@@ -2511,8 +2902,23 @@
       <c r="K3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="6">
+        <v>479</v>
+      </c>
+      <c r="M3" s="7">
+        <f>Tabelle145[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>143.69999999999999</v>
+      </c>
+      <c r="N3" s="8">
+        <f>$N$2</f>
+        <v>1.02</v>
+      </c>
+      <c r="O3" s="5">
+        <f>ROUND((Tabelle145[[#This Row],[Kosten Straße CHF/m]]+Tabelle145[[#This Row],[Aufschlag (30%)]])*Tabelle145[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>635.15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>172</v>
       </c>
@@ -2546,8 +2952,23 @@
       <c r="K4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="7">
+        <v>511</v>
+      </c>
+      <c r="M4" s="7">
+        <f>Tabelle145[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>153.29999999999998</v>
+      </c>
+      <c r="N4" s="8">
+        <f t="shared" ref="N4:N23" si="0">$N$2</f>
+        <v>1.02</v>
+      </c>
+      <c r="O4" s="5">
+        <f>ROUND((Tabelle145[[#This Row],[Kosten Straße CHF/m]]+Tabelle145[[#This Row],[Aufschlag (30%)]])*Tabelle145[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>677.59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>175</v>
       </c>
@@ -2581,8 +3002,23 @@
       <c r="K5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="7">
+        <v>529</v>
+      </c>
+      <c r="M5" s="7">
+        <f>Tabelle145[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>158.69999999999999</v>
+      </c>
+      <c r="N5" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O5" s="5">
+        <f>ROUND((Tabelle145[[#This Row],[Kosten Straße CHF/m]]+Tabelle145[[#This Row],[Aufschlag (30%)]])*Tabelle145[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>701.45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>177</v>
       </c>
@@ -2616,8 +3052,23 @@
       <c r="K6" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="7">
+        <v>599</v>
+      </c>
+      <c r="M6" s="7">
+        <f>Tabelle145[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>179.7</v>
+      </c>
+      <c r="N6" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O6" s="5">
+        <f>ROUND((Tabelle145[[#This Row],[Kosten Straße CHF/m]]+Tabelle145[[#This Row],[Aufschlag (30%)]])*Tabelle145[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>794.27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>181</v>
       </c>
@@ -2651,8 +3102,23 @@
       <c r="K7" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="7">
+        <v>650</v>
+      </c>
+      <c r="M7" s="7">
+        <f>Tabelle145[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>195</v>
+      </c>
+      <c r="N7" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O7" s="5">
+        <f>ROUND((Tabelle145[[#This Row],[Kosten Straße CHF/m]]+Tabelle145[[#This Row],[Aufschlag (30%)]])*Tabelle145[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>861.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>184</v>
       </c>
@@ -2686,8 +3152,23 @@
       <c r="K8" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="7">
+        <v>745</v>
+      </c>
+      <c r="M8" s="7">
+        <f>Tabelle145[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>223.5</v>
+      </c>
+      <c r="N8" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O8" s="5">
+        <f>ROUND((Tabelle145[[#This Row],[Kosten Straße CHF/m]]+Tabelle145[[#This Row],[Aufschlag (30%)]])*Tabelle145[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>987.87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>188</v>
       </c>
@@ -2721,8 +3202,23 @@
       <c r="K9" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="7">
+        <v>920</v>
+      </c>
+      <c r="M9" s="7">
+        <f>Tabelle145[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>276</v>
+      </c>
+      <c r="N9" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O9" s="5">
+        <f>ROUND((Tabelle145[[#This Row],[Kosten Straße CHF/m]]+Tabelle145[[#This Row],[Aufschlag (30%)]])*Tabelle145[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>1219.92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>169</v>
       </c>
@@ -2756,8 +3252,23 @@
       <c r="K10" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="7">
+        <v>1105</v>
+      </c>
+      <c r="M10" s="7">
+        <f>Tabelle145[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>331.5</v>
+      </c>
+      <c r="N10" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O10" s="5">
+        <f>ROUND((Tabelle145[[#This Row],[Kosten Straße CHF/m]]+Tabelle145[[#This Row],[Aufschlag (30%)]])*Tabelle145[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>1465.23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>194</v>
       </c>
@@ -2791,8 +3302,23 @@
       <c r="K11" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="7">
+        <v>1332</v>
+      </c>
+      <c r="M11" s="7">
+        <f>Tabelle145[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>399.59999999999997</v>
+      </c>
+      <c r="N11" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O11" s="5">
+        <f>ROUND((Tabelle145[[#This Row],[Kosten Straße CHF/m]]+Tabelle145[[#This Row],[Aufschlag (30%)]])*Tabelle145[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>1766.23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>187</v>
       </c>
@@ -2826,8 +3352,23 @@
       <c r="K12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="7">
+        <v>1586</v>
+      </c>
+      <c r="M12" s="7">
+        <f>Tabelle145[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>475.79999999999995</v>
+      </c>
+      <c r="N12" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O12" s="5">
+        <f>ROUND((Tabelle145[[#This Row],[Kosten Straße CHF/m]]+Tabelle145[[#This Row],[Aufschlag (30%)]])*Tabelle145[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>2103.04</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>192</v>
       </c>
@@ -2861,8 +3402,23 @@
       <c r="K13" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" s="7">
+        <v>2124</v>
+      </c>
+      <c r="M13" s="7">
+        <f>Tabelle145[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>637.19999999999993</v>
+      </c>
+      <c r="N13" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O13" s="5">
+        <f>ROUND((Tabelle145[[#This Row],[Kosten Straße CHF/m]]+Tabelle145[[#This Row],[Aufschlag (30%)]])*Tabelle145[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>2816.42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>300</v>
       </c>
@@ -2896,8 +3452,23 @@
       <c r="K14" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="7">
+        <v>2662</v>
+      </c>
+      <c r="M14" s="7">
+        <f>Tabelle145[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>798.6</v>
+      </c>
+      <c r="N14" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O14" s="5">
+        <f>ROUND((Tabelle145[[#This Row],[Kosten Straße CHF/m]]+Tabelle145[[#This Row],[Aufschlag (30%)]])*Tabelle145[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>3529.81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>350</v>
       </c>
@@ -2931,8 +3502,23 @@
       <c r="K15" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" s="7">
+        <v>3200</v>
+      </c>
+      <c r="M15" s="7">
+        <f>Tabelle145[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>960</v>
+      </c>
+      <c r="N15" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O15" s="5">
+        <f>ROUND((Tabelle145[[#This Row],[Kosten Straße CHF/m]]+Tabelle145[[#This Row],[Aufschlag (30%)]])*Tabelle145[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>4243.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>400</v>
       </c>
@@ -2966,8 +3552,23 @@
       <c r="K16" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L16" s="7">
+        <v>3738</v>
+      </c>
+      <c r="M16" s="7">
+        <f>Tabelle145[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>1121.3999999999999</v>
+      </c>
+      <c r="N16" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O16" s="5">
+        <f>ROUND((Tabelle145[[#This Row],[Kosten Straße CHF/m]]+Tabelle145[[#This Row],[Aufschlag (30%)]])*Tabelle145[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>4956.59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>450</v>
       </c>
@@ -3001,8 +3602,23 @@
       <c r="K17" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L17" s="7">
+        <v>4276</v>
+      </c>
+      <c r="M17" s="7">
+        <f>Tabelle145[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>1282.8</v>
+      </c>
+      <c r="N17" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O17" s="5">
+        <f>ROUND((Tabelle145[[#This Row],[Kosten Straße CHF/m]]+Tabelle145[[#This Row],[Aufschlag (30%)]])*Tabelle145[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>5669.98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>500</v>
       </c>
@@ -3036,8 +3652,23 @@
       <c r="K18" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L18" s="7">
+        <v>4814</v>
+      </c>
+      <c r="M18" s="7">
+        <f>Tabelle145[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>1444.2</v>
+      </c>
+      <c r="N18" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O18" s="5">
+        <f>ROUND((Tabelle145[[#This Row],[Kosten Straße CHF/m]]+Tabelle145[[#This Row],[Aufschlag (30%)]])*Tabelle145[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>6383.36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>600</v>
       </c>
@@ -3071,8 +3702,23 @@
       <c r="K19" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L19" s="7">
+        <v>5352</v>
+      </c>
+      <c r="M19" s="7">
+        <f>Tabelle145[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>1605.6</v>
+      </c>
+      <c r="N19" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O19" s="5">
+        <f>ROUND((Tabelle145[[#This Row],[Kosten Straße CHF/m]]+Tabelle145[[#This Row],[Aufschlag (30%)]])*Tabelle145[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>7096.75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>217</v>
       </c>
@@ -3106,10 +3752,23 @@
       <c r="K20" t="s">
         <v>143</v>
       </c>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L20" s="7">
+        <v>5890</v>
+      </c>
+      <c r="M20" s="7">
+        <f>Tabelle145[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>1767</v>
+      </c>
+      <c r="N20" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O20" s="5">
+        <f>ROUND((Tabelle145[[#This Row],[Kosten Straße CHF/m]]+Tabelle145[[#This Row],[Aufschlag (30%)]])*Tabelle145[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>7810.14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>210</v>
       </c>
@@ -3143,10 +3802,23 @@
       <c r="K21" t="s">
         <v>147</v>
       </c>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L21" s="7">
+        <v>6428</v>
+      </c>
+      <c r="M21" s="7">
+        <f>Tabelle145[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>1928.3999999999999</v>
+      </c>
+      <c r="N21" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O21" s="5">
+        <f>ROUND((Tabelle145[[#This Row],[Kosten Straße CHF/m]]+Tabelle145[[#This Row],[Aufschlag (30%)]])*Tabelle145[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>8523.5300000000007</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>212</v>
       </c>
@@ -3180,10 +3852,23 @@
       <c r="K22" t="s">
         <v>33</v>
       </c>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L22" s="7">
+        <v>6966</v>
+      </c>
+      <c r="M22" s="7">
+        <f>Tabelle145[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>2089.7999999999997</v>
+      </c>
+      <c r="N22" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O22" s="5">
+        <f>ROUND((Tabelle145[[#This Row],[Kosten Straße CHF/m]]+Tabelle145[[#This Row],[Aufschlag (30%)]])*Tabelle145[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>9236.92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>215</v>
       </c>
@@ -3217,8 +3902,21 @@
       <c r="K23" t="s">
         <v>33</v>
       </c>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
+      <c r="L23" s="7">
+        <v>7504</v>
+      </c>
+      <c r="M23" s="7">
+        <f>Tabelle145[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>2251.1999999999998</v>
+      </c>
+      <c r="N23" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O23" s="5">
+        <f>ROUND((Tabelle145[[#This Row],[Kosten Straße CHF/m]]+Tabelle145[[#This Row],[Aufschlag (30%)]])*Tabelle145[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>9950.2999999999993</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3230,10 +3928,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E844A536-D923-41BD-9435-2FBAB590FD2D}">
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3244,9 +3942,13 @@
     <col min="4" max="4" width="19.42578125" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" customWidth="1"/>
     <col min="6" max="11" width="12.140625" customWidth="1"/>
+    <col min="12" max="12" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>270</v>
       </c>
@@ -3280,8 +3982,20 @@
       <c r="K1" s="4" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>164</v>
       </c>
@@ -3315,8 +4029,22 @@
       <c r="K2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="6">
+        <v>374</v>
+      </c>
+      <c r="M2" s="7">
+        <f>Tabelle14[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>112.2</v>
+      </c>
+      <c r="N2" s="8">
+        <v>1.02</v>
+      </c>
+      <c r="O2" s="5">
+        <f>ROUND((Tabelle14[[#This Row],[Kosten Straße CHF/m]]+Tabelle14[[#This Row],[Aufschlag (30%)]])*Tabelle14[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>495.92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>170</v>
       </c>
@@ -3350,8 +4078,23 @@
       <c r="K3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="6">
+        <v>378</v>
+      </c>
+      <c r="M3" s="7">
+        <f>Tabelle14[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>113.39999999999999</v>
+      </c>
+      <c r="N3" s="8">
+        <f>$N$2</f>
+        <v>1.02</v>
+      </c>
+      <c r="O3" s="5">
+        <f>ROUND((Tabelle14[[#This Row],[Kosten Straße CHF/m]]+Tabelle14[[#This Row],[Aufschlag (30%)]])*Tabelle14[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>501.23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>172</v>
       </c>
@@ -3385,8 +4128,23 @@
       <c r="K4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="7">
+        <v>404</v>
+      </c>
+      <c r="M4" s="7">
+        <f>Tabelle14[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>121.19999999999999</v>
+      </c>
+      <c r="N4" s="8">
+        <f t="shared" ref="N4:N12" si="0">$N$2</f>
+        <v>1.02</v>
+      </c>
+      <c r="O4" s="5">
+        <f>ROUND((Tabelle14[[#This Row],[Kosten Straße CHF/m]]+Tabelle14[[#This Row],[Aufschlag (30%)]])*Tabelle14[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>535.70000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>175</v>
       </c>
@@ -3420,8 +4178,23 @@
       <c r="K5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="7">
+        <v>418</v>
+      </c>
+      <c r="M5" s="7">
+        <f>Tabelle14[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>125.39999999999999</v>
+      </c>
+      <c r="N5" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O5" s="5">
+        <f>ROUND((Tabelle14[[#This Row],[Kosten Straße CHF/m]]+Tabelle14[[#This Row],[Aufschlag (30%)]])*Tabelle14[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>554.27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>177</v>
       </c>
@@ -3455,8 +4228,23 @@
       <c r="K6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="7">
+        <v>473</v>
+      </c>
+      <c r="M6" s="7">
+        <f>Tabelle14[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>141.9</v>
+      </c>
+      <c r="N6" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O6" s="5">
+        <f>ROUND((Tabelle14[[#This Row],[Kosten Straße CHF/m]]+Tabelle14[[#This Row],[Aufschlag (30%)]])*Tabelle14[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>627.20000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>181</v>
       </c>
@@ -3490,8 +4278,23 @@
       <c r="K7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="7">
+        <v>514</v>
+      </c>
+      <c r="M7" s="7">
+        <f>Tabelle14[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>154.19999999999999</v>
+      </c>
+      <c r="N7" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O7" s="5">
+        <f>ROUND((Tabelle14[[#This Row],[Kosten Straße CHF/m]]+Tabelle14[[#This Row],[Aufschlag (30%)]])*Tabelle14[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>681.56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>184</v>
       </c>
@@ -3525,8 +4328,23 @@
       <c r="K8" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="7">
+        <v>589</v>
+      </c>
+      <c r="M8" s="7">
+        <f>Tabelle14[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>176.7</v>
+      </c>
+      <c r="N8" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O8" s="5">
+        <f>ROUND((Tabelle14[[#This Row],[Kosten Straße CHF/m]]+Tabelle14[[#This Row],[Aufschlag (30%)]])*Tabelle14[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>781.01</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>188</v>
       </c>
@@ -3560,8 +4378,23 @@
       <c r="K9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="7">
+        <v>727</v>
+      </c>
+      <c r="M9" s="7">
+        <f>Tabelle14[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>218.1</v>
+      </c>
+      <c r="N9" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O9" s="5">
+        <f>ROUND((Tabelle14[[#This Row],[Kosten Straße CHF/m]]+Tabelle14[[#This Row],[Aufschlag (30%)]])*Tabelle14[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>964</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>169</v>
       </c>
@@ -3595,8 +4428,23 @@
       <c r="K10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="7">
+        <v>873</v>
+      </c>
+      <c r="M10" s="7">
+        <f>Tabelle14[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>261.89999999999998</v>
+      </c>
+      <c r="N10" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O10" s="5">
+        <f>ROUND((Tabelle14[[#This Row],[Kosten Straße CHF/m]]+Tabelle14[[#This Row],[Aufschlag (30%)]])*Tabelle14[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>1157.5999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>194</v>
       </c>
@@ -3630,8 +4478,23 @@
       <c r="K11" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="7">
+        <v>1052</v>
+      </c>
+      <c r="M11" s="7">
+        <f>Tabelle14[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>315.59999999999997</v>
+      </c>
+      <c r="N11" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O11" s="5">
+        <f>ROUND((Tabelle14[[#This Row],[Kosten Straße CHF/m]]+Tabelle14[[#This Row],[Aufschlag (30%)]])*Tabelle14[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>1394.95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>187</v>
       </c>
@@ -3665,8 +4528,23 @@
       <c r="K12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="7">
+        <v>1253</v>
+      </c>
+      <c r="M12" s="7">
+        <f>Tabelle14[[#This Row],[Kosten Straße CHF/m]]*0.3</f>
+        <v>375.9</v>
+      </c>
+      <c r="N12" s="8">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="O12" s="5">
+        <f>ROUND((Tabelle14[[#This Row],[Kosten Straße CHF/m]]+Tabelle14[[#This Row],[Aufschlag (30%)]])*Tabelle14[[#This Row],[Umrechnung CHF in €]],2)</f>
+        <v>1661.48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>

</xml_diff>